<commit_message>
Updated column header of Excel
</commit_message>
<xml_diff>
--- a/HydroBOSSE/project_List_30MW.xlsx
+++ b/HydroBOSSE/project_List_30MW.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpoudel\PycharmProjects\hybrids_shared_infrastructure\HydroBOSSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C77530E-AC63-4E9D-B3FB-B75F294B3525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2009A6-99B9-473E-A04E-FC2D4E064265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{0D60E450-1675-450E-BD0E-8D35825305C1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="5" r:id="rId1"/>
-    <sheet name="USACost" sheetId="6" r:id="rId2"/>
-    <sheet name="LCMCosts" sheetId="8" r:id="rId3"/>
+    <sheet name="metadata" sheetId="5" r:id="rId1"/>
+    <sheet name="usacost_df" sheetId="6" r:id="rId2"/>
+    <sheet name="lcmcosts_df" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="AEP">Metadata!$B$22</definedName>
-    <definedName name="capacityfactor">Metadata!$B$20</definedName>
-    <definedName name="H_">Metadata!$B$19</definedName>
-    <definedName name="hours_year">Metadata!$B$21</definedName>
-    <definedName name="P_">Metadata!$B$13</definedName>
+    <definedName name="AEP">metadata!$X$2</definedName>
+    <definedName name="capacityfactor">metadata!$U$2</definedName>
+    <definedName name="H_">metadata!$T$2</definedName>
+    <definedName name="hours_year">metadata!$W$2</definedName>
+    <definedName name="P_">metadata!$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,70 +42,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={E900306C-E723-4FC2-9497-DD9B646AB063}</author>
-    <author>tc={60659B67-43D6-4A0A-8928-22E6C5D28B52}</author>
-    <author>tc={A7EF4123-AAF4-4998-B0A1-7C867F6E7C04}</author>
-    <author>tc={5FB9FAB0-163A-4E27-8B16-01384BB7920A}</author>
-    <author>tc={E3C97F59-AB41-42B1-B161-03B5D72A4B46}</author>
-    <author>tc={11123E3A-39EB-457B-8A83-08DB00C18395}</author>
-  </authors>
-  <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{E900306C-E723-4FC2-9497-DD9B646AB063}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Project Name</t>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="1" shapeId="0" xr:uid="{60659B67-43D6-4A0A-8928-22E6C5D28B52}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    North American Electric Reliability Corporation</t>
-      </text>
-    </comment>
-    <comment ref="A11" authorId="2" shapeId="0" xr:uid="{A7EF4123-AAF4-4998-B0A1-7C867F6E7C04}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Owner classcode: Cooperative (C); Federal (F); Industrial (I); Municipal (M) and other non-federal; Private Utility(P); Private non-utility</t>
-      </text>
-    </comment>
-    <comment ref="A17" authorId="3" shapeId="0" xr:uid="{5FB9FAB0-163A-4E27-8B16-01384BB7920A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Status of Dam (W = With Power, W/O = Without Power, U = Undeveloped)</t>
-      </text>
-    </comment>
-    <comment ref="B25" authorId="4" shapeId="0" xr:uid="{E3C97F59-AB41-42B1-B161-03B5D72A4B46}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Conception to Commercial Production time in Years</t>
-      </text>
-    </comment>
-    <comment ref="A28" authorId="5" shapeId="0" xr:uid="{11123E3A-39EB-457B-8A83-08DB00C18395}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Aggregate cost infation based on the cost base year and current year. Use CCT unless otherwise stated.
-'=function (Year Commision, Year Cost Model, Year Analysis)</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={1E9BD81B-0BB7-4D0E-ACC6-D433A2855831}</author>
@@ -205,13 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="164">
-  <si>
-    <t>Project No</t>
-  </si>
-  <si>
-    <t>StreamName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="159">
   <si>
     <t>State</t>
   </si>
@@ -225,45 +155,15 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>ClassCode</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
-    <t>Capacity</t>
-  </si>
-  <si>
-    <t>UnitType</t>
-  </si>
-  <si>
-    <t>PlantType</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
-    <t>PlantName</t>
-  </si>
-  <si>
-    <t>BasinName</t>
-  </si>
-  <si>
-    <t>Head</t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>CapacityFactor(Yearly)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.25 &lt; x &lt; 0.85</t>
   </si>
   <si>
-    <t>Some Example Projects</t>
-  </si>
-  <si>
     <t>Licensing - Undeveloped Sites</t>
   </si>
   <si>
@@ -357,33 +257,6 @@
     <t>CostCode</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
     <t>1.1.2 Dams and Reservoirs</t>
   </si>
   <si>
@@ -456,21 +329,12 @@
     <t>Generator Rewind projects</t>
   </si>
   <si>
-    <t>AEP</t>
-  </si>
-  <si>
-    <t>MWh</t>
-  </si>
-  <si>
     <t>NSD/kW</t>
   </si>
   <si>
     <t xml:space="preserve">1.2.1 Development </t>
   </si>
   <si>
-    <t xml:space="preserve">FERC: accelerated development schedule </t>
-  </si>
-  <si>
     <t>1.1.4 Powerhouse Structures (and shaft)</t>
   </si>
   <si>
@@ -486,12 +350,6 @@
     <t>%ICC(woFC)</t>
   </si>
   <si>
-    <t>ConstructionTotal project construction time (months)</t>
-  </si>
-  <si>
-    <t>months</t>
-  </si>
-  <si>
     <t>npd</t>
   </si>
   <si>
@@ -585,24 +443,12 @@
     <t>var_oam</t>
   </si>
   <si>
-    <t>meter</t>
-  </si>
-  <si>
-    <t>https://www.usbr.gov/power/data/faclname.html</t>
-  </si>
-  <si>
-    <t>Project Metadata and Specification</t>
-  </si>
-  <si>
     <t>uid</t>
   </si>
   <si>
     <t>CostModelYear</t>
   </si>
   <si>
-    <t>CostEscalation</t>
-  </si>
-  <si>
     <t>CostEscalationFactor</t>
   </si>
   <si>
@@ -624,12 +470,6 @@
     <t>CostUSD</t>
   </si>
   <si>
-    <t>YearCommision</t>
-  </si>
-  <si>
-    <t>YearAnalysis</t>
-  </si>
-  <si>
     <t>Blue River</t>
   </si>
   <si>
@@ -654,30 +494,12 @@
     <t>Rocky Mountain Power Area</t>
   </si>
   <si>
-    <t>km^2</t>
-  </si>
-  <si>
     <t>USBR</t>
   </si>
   <si>
     <t>21 km (13 miles)</t>
   </si>
   <si>
-    <t>Missouri Basin(?)</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>hour</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1.1Generating Plant</t>
   </si>
   <si>
@@ -693,10 +515,109 @@
     <t>2.0 Sub-Total Cost</t>
   </si>
   <si>
-    <t>DamStatus</t>
-  </si>
-  <si>
-    <t>Hours_per_Year</t>
+    <t>NERC Area</t>
+  </si>
+  <si>
+    <t>AEP (MWh)</t>
+  </si>
+  <si>
+    <t>Cost escalation</t>
+  </si>
+  <si>
+    <t>Year analysis</t>
+  </si>
+  <si>
+    <t>Total project construction time (months)</t>
+  </si>
+  <si>
+    <t>Generator RPM range</t>
+  </si>
+  <si>
+    <t>Hours per year</t>
+  </si>
+  <si>
+    <t>Capacity factor (yearly)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dam length </t>
+  </si>
+  <si>
+    <t>Dam status</t>
+  </si>
+  <si>
+    <t>with power</t>
+  </si>
+  <si>
+    <t>Capacity (MW)</t>
+  </si>
+  <si>
+    <t>Head (meter)</t>
+  </si>
+  <si>
+    <t>Capacity factor range</t>
+  </si>
+  <si>
+    <t>Basin size (km2)</t>
+  </si>
+  <si>
+    <t>Owner classcode</t>
+  </si>
+  <si>
+    <t>Municipal</t>
+  </si>
+  <si>
+    <t>Project no</t>
+  </si>
+  <si>
+    <t>Project name</t>
+  </si>
+  <si>
+    <t>Basin name</t>
+  </si>
+  <si>
+    <t>Stream name</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Unit type</t>
+  </si>
+  <si>
+    <t>Plant type</t>
+  </si>
+  <si>
+    <t>Year commision</t>
+  </si>
+  <si>
+    <t>Missouri Basin</t>
+  </si>
+  <si>
+    <t>Collection</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>Grid Connection</t>
+  </si>
+  <si>
+    <t>HydropBost</t>
+  </si>
+  <si>
+    <t>InverterTransformer Erection</t>
+  </si>
+  <si>
+    <t>Management Cost</t>
+  </si>
+  <si>
+    <t>Racking System Installation</t>
+  </si>
+  <si>
+    <t>Site Prepartion</t>
+  </si>
+  <si>
+    <t>Substation Cost</t>
   </si>
 </sst>
 </file>
@@ -709,18 +630,10 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -880,13 +793,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -907,7 +818,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -935,28 +846,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1275,30 +1178,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A3" dT="2020-07-08T15:10:10.51" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{E900306C-E723-4FC2-9497-DD9B646AB063}">
-    <text>Project Name</text>
-  </threadedComment>
-  <threadedComment ref="A7" dT="2020-07-07T19:45:13.82" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{60659B67-43D6-4A0A-8928-22E6C5D28B52}">
-    <text>North American Electric Reliability Corporation</text>
-  </threadedComment>
-  <threadedComment ref="A11" dT="2020-07-07T21:29:44.64" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{A7EF4123-AAF4-4998-B0A1-7C867F6E7C04}">
-    <text>Owner classcode: Cooperative (C); Federal (F); Industrial (I); Municipal (M) and other non-federal; Private Utility(P); Private non-utility</text>
-  </threadedComment>
-  <threadedComment ref="A17" dT="2020-07-07T22:30:06.08" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{5FB9FAB0-163A-4E27-8B16-01384BB7920A}">
-    <text>Status of Dam (W = With Power, W/O = Without Power, U = Undeveloped)</text>
-  </threadedComment>
-  <threadedComment ref="B25" dT="2020-07-22T20:48:28.98" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{E3C97F59-AB41-42B1-B161-03B5D72A4B46}">
-    <text>Conception to Commercial Production time in Years</text>
-  </threadedComment>
-  <threadedComment ref="A28" dT="2020-07-15T15:46:38.57" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{11123E3A-39EB-457B-8A83-08DB00C18395}">
-    <text>Aggregate cost infation based on the cost base year and current year. Use CCT unless otherwise stated.
-'=function (Year Commision, Year Cost Model, Year Analysis)</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="F1" dT="2020-07-21T22:26:12.19" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{1E9BD81B-0BB7-4D0E-ACC6-D433A2855831}">
     <text>Best guess after separating the Financial Cost; Screen shot below -original % based on multiple data source</text>
   </threadedComment>
@@ -1333,273 +1212,201 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B91564F-1603-4DC5-B4A2-6AD0B294541F}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B91564F-1603-4DC5-B4A2-6AD0B294541F}">
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>147</v>
+      </c>
+      <c r="R1" t="s">
+        <v>133</v>
+      </c>
+      <c r="S1" t="s">
+        <v>132</v>
+      </c>
+      <c r="T1" t="s">
+        <v>136</v>
+      </c>
+      <c r="U1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" t="s">
+        <v>130</v>
+      </c>
+      <c r="X1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA1" t="s">
         <v>128</v>
       </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
+      <c r="AB1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4">
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2">
         <v>1800</v>
       </c>
-      <c r="D4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2">
+        <v>1984</v>
+      </c>
+      <c r="K2">
         <v>39.878725000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
+      <c r="L2">
         <v>-106.33275999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="M2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O2">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" t="s">
+        <v>134</v>
+      </c>
+      <c r="S2" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2">
+        <v>64</v>
+      </c>
+      <c r="U2">
+        <v>0.6</v>
+      </c>
+      <c r="V2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C17" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>64</v>
-      </c>
-      <c r="D19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>0.6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>163</v>
-      </c>
-      <c r="B21">
-        <f>24*365</f>
+      <c r="W2">
         <v>8760</v>
       </c>
-      <c r="D21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22">
-        <f>P_*0.6*8760</f>
+      <c r="X2">
         <v>136656</v>
       </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23">
+      <c r="Y2">
         <v>1000</v>
       </c>
-      <c r="C23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25">
-        <f>8.5*12</f>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2">
         <v>102</v>
       </c>
-      <c r="D25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>139</v>
-      </c>
-      <c r="B26">
+      <c r="AB2">
         <v>1943</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>140</v>
-      </c>
-      <c r="B27">
-        <f ca="1">YEAR(TODAY())</f>
+      <c r="AC2">
         <v>2020</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>131</v>
-      </c>
-      <c r="B28">
+      <c r="AD2">
         <v>1.03</v>
-      </c>
-      <c r="C28" s="37"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1608,7 +1415,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,906 +1428,906 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="14" t="s">
+      <c r="A1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" s="10"/>
+      <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O1" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q1" s="9"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="17">
+      <c r="A2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="16">
         <v>2</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="17">
         <v>110</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="30">
         <f>SUM(D3:D9)</f>
         <v>56.999999999999993</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="27">
         <f>SUM(E3:E9)</f>
         <v>2686.87</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <f>SUM(F3:F9)</f>
         <v>62.79</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="27">
         <f t="shared" ref="G2:G18" si="0">F2*$G$25/100</f>
         <v>3063.2535704576371</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="36"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="33"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="20">
+      <c r="A3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="19">
         <v>3</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <v>111</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="31">
         <v>3.27</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="26">
         <v>154.07</v>
       </c>
       <c r="F3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="26">
         <f>F3*$G$25/100</f>
         <v>224.41418098590748</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26">
-        <v>0</v>
-      </c>
-      <c r="O3" s="26">
+      <c r="H3" s="31"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25">
+        <v>0</v>
+      </c>
+      <c r="O3" s="25">
         <v>1</v>
       </c>
-      <c r="P3" s="27"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="22">
+      <c r="A4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="21">
         <v>3</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>112</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <v>19.079999999999998</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <v>899.31</v>
       </c>
       <c r="F4">
         <v>16.850000000000001</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="26">
         <f t="shared" si="0"/>
         <v>822.03890208968301</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="26">
+      <c r="H4" s="31"/>
+      <c r="I4" s="25">
         <v>1</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26">
-        <v>0</v>
-      </c>
-      <c r="O4" s="26"/>
-      <c r="P4" s="27"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25">
+        <v>0</v>
+      </c>
+      <c r="O4" s="25"/>
+      <c r="P4" s="26"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="22">
+      <c r="A5" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="21">
         <v>3</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <v>113</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <v>2.98</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <v>140.66999999999999</v>
       </c>
       <c r="F5">
         <v>4.5199999999999996</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <f t="shared" si="0"/>
         <v>220.51132566441342</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26">
-        <v>0</v>
-      </c>
-      <c r="O5" s="26"/>
-      <c r="P5" s="27"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25">
+        <v>0</v>
+      </c>
+      <c r="O5" s="25"/>
+      <c r="P5" s="26"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="22">
+      <c r="A6" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="21">
         <v>3</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>114</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>10.37</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <v>489.01</v>
       </c>
       <c r="F6">
         <v>14.6</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="26">
         <f t="shared" si="0"/>
         <v>712.27109617266285</v>
       </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26">
-        <v>0</v>
-      </c>
-      <c r="O6" s="26"/>
-      <c r="P6" s="27"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25">
+        <v>0</v>
+      </c>
+      <c r="O6" s="25"/>
+      <c r="P6" s="26"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="23">
+      <c r="A7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="22">
         <v>3</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="20">
         <v>115</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>11.65</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>549.29999999999995</v>
       </c>
       <c r="F7">
         <v>13.4</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="26">
         <f t="shared" si="0"/>
         <v>653.72826635025228</v>
       </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26">
-        <v>0</v>
-      </c>
-      <c r="O7" s="26"/>
-      <c r="P7" s="27"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25">
+        <v>0</v>
+      </c>
+      <c r="O7" s="25"/>
+      <c r="P7" s="26"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="23">
+      <c r="A8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="22">
         <v>3</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>116</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>7.11</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <v>334.94</v>
       </c>
       <c r="F8">
         <v>5.25</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="26">
         <f t="shared" si="0"/>
         <v>256.12488047304657</v>
       </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26">
+      <c r="H8" s="31"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25">
         <v>1</v>
       </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26">
-        <v>0</v>
-      </c>
-      <c r="O8" s="26"/>
-      <c r="P8" s="27"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25">
+        <v>0</v>
+      </c>
+      <c r="O8" s="25"/>
+      <c r="P8" s="26"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="23">
+      <c r="A9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="22">
         <v>3</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <v>117</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>2.54</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <v>119.57</v>
       </c>
       <c r="F9">
         <v>3.57</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="26">
         <f t="shared" si="0"/>
         <v>174.16491872167168</v>
       </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26">
-        <v>0</v>
-      </c>
-      <c r="O9" s="26"/>
-      <c r="P9" s="27"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25">
+        <v>0</v>
+      </c>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="17">
+      <c r="A10" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="16">
         <v>2</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>120</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <f>SUM(D11:D18)</f>
         <v>20</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <f>SUM(E11:E18)</f>
         <v>942.75999999999988</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f>SUM(F11:F18)</f>
         <v>37.22</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="27">
         <f t="shared" si="0"/>
         <v>1815.8034383251036</v>
       </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29">
+      <c r="H10" s="30"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28">
         <v>1</v>
       </c>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="27"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="22">
+      <c r="A11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="21">
         <v>3</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="20">
         <v>121</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <v>2.12</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="26">
         <v>99.84</v>
       </c>
       <c r="F11">
         <v>5</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="26">
         <f t="shared" si="0"/>
         <v>243.92845759337769</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26">
-        <v>0</v>
-      </c>
-      <c r="O11" s="26">
+      <c r="H11" s="31"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25">
+        <v>0</v>
+      </c>
+      <c r="O11" s="25">
         <v>0.12</v>
       </c>
-      <c r="P11" s="27"/>
+      <c r="P11" s="26"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="20">
+      <c r="A12" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="19">
         <v>3</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>122</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <v>9.85</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="26">
         <v>464.08</v>
       </c>
       <c r="F12">
         <v>13.8</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <f t="shared" si="0"/>
         <v>673.24254295772243</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26">
+      <c r="H12" s="31"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25">
         <v>1</v>
       </c>
-      <c r="N12" s="26">
-        <v>0</v>
-      </c>
-      <c r="O12" s="26"/>
-      <c r="P12" s="27"/>
+      <c r="N12" s="25">
+        <v>0</v>
+      </c>
+      <c r="O12" s="25"/>
+      <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="24">
+      <c r="A13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="23">
         <v>3</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>123</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <v>1.99</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="26">
         <v>93.85</v>
       </c>
       <c r="F13">
         <v>4.7</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <f t="shared" si="0"/>
         <v>229.29275013777504</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="31">
         <v>1</v>
       </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26">
+      <c r="I13" s="25"/>
+      <c r="J13" s="25">
         <v>1</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26">
+      <c r="K13" s="25"/>
+      <c r="L13" s="25">
         <v>1</v>
       </c>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26">
-        <v>0</v>
-      </c>
-      <c r="O13" s="26"/>
-      <c r="P13" s="27">
+      <c r="M13" s="25"/>
+      <c r="N13" s="25">
+        <v>0</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="P13" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="23">
+      <c r="A14" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="22">
         <v>3</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <v>124</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="31">
         <v>0.64</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="26">
         <v>29.93</v>
       </c>
       <c r="F14">
         <v>1.5</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="26">
         <f t="shared" si="0"/>
         <v>73.178537278013309</v>
       </c>
-      <c r="H14" s="32"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26">
+      <c r="H14" s="31"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25">
         <v>1</v>
       </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26">
+      <c r="K14" s="25"/>
+      <c r="L14" s="25">
         <v>1</v>
       </c>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26">
-        <v>0</v>
-      </c>
-      <c r="O14" s="26"/>
-      <c r="P14" s="27"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25">
+        <v>0</v>
+      </c>
+      <c r="O14" s="25"/>
+      <c r="P14" s="26"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="22">
+      <c r="A15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="21">
         <v>3</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <v>125</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="31">
         <v>1.02</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <v>48.13</v>
       </c>
       <c r="F15">
         <v>2.41</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="26">
         <f t="shared" si="0"/>
         <v>117.57351656000806</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26">
-        <v>0</v>
-      </c>
-      <c r="O15" s="26">
+      <c r="H15" s="31"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25">
+        <v>0</v>
+      </c>
+      <c r="O15" s="25">
         <v>1</v>
       </c>
-      <c r="P15" s="27"/>
+      <c r="P15" s="26"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="25">
+      <c r="A16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="24">
         <v>3</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <v>126</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <v>0.21</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="26">
         <v>9.99</v>
       </c>
       <c r="F16">
         <v>0.5</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="26">
         <f t="shared" si="0"/>
         <v>24.392845759337771</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26">
+      <c r="H16" s="31"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25">
         <v>1</v>
       </c>
-      <c r="N16" s="26">
-        <v>0</v>
-      </c>
-      <c r="O16" s="26"/>
-      <c r="P16" s="27"/>
+      <c r="N16" s="25">
+        <v>0</v>
+      </c>
+      <c r="O16" s="25"/>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="22">
+      <c r="A17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="21">
         <v>3</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="20">
         <v>127</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>3.95</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="26">
         <v>186.38</v>
       </c>
       <c r="F17">
         <v>8.7799999999999994</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="26">
         <f t="shared" si="0"/>
         <v>428.33837153397121</v>
       </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26">
-        <v>0</v>
-      </c>
-      <c r="O17" s="26">
+      <c r="H17" s="31"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25">
+        <v>0</v>
+      </c>
+      <c r="O17" s="25">
         <v>1</v>
       </c>
-      <c r="P17" s="27"/>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="22">
+      <c r="A18" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="21">
         <v>3</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="20">
         <v>128</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <v>0.22</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="26">
         <v>10.56</v>
       </c>
       <c r="F18">
         <v>0.53</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="26">
         <f t="shared" si="0"/>
         <v>25.856416504898039</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26">
-        <v>0</v>
-      </c>
-      <c r="O18" s="26">
+      <c r="H18" s="31"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25">
+        <v>0</v>
+      </c>
+      <c r="O18" s="25">
         <v>0.1</v>
       </c>
-      <c r="P18" s="27"/>
+      <c r="P18" s="26"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="B19" s="17">
+      <c r="A19" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="16">
         <v>2</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="17">
         <v>130</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="30">
         <f>SUM(D20:D24)</f>
         <v>22.95</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="27">
         <f>SUM(E20:E24)</f>
         <v>1081.8400000000001</v>
       </c>
-      <c r="F19" s="31">
-        <v>0</v>
-      </c>
-      <c r="G19" s="28">
-        <v>0</v>
-      </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="28"/>
+      <c r="F19" s="30">
+        <v>0</v>
+      </c>
+      <c r="G19" s="27">
+        <v>0</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="27"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="25">
+      <c r="A20" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="24">
         <v>3</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="20">
         <v>131</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="31">
         <v>3.8</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="26">
         <v>179.13</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26">
-        <v>0</v>
-      </c>
-      <c r="O20" s="26"/>
-      <c r="P20" s="27"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25">
+        <v>0</v>
+      </c>
+      <c r="O20" s="25"/>
+      <c r="P20" s="26"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="25">
+      <c r="A21" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="24">
         <v>3</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <v>132</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="31">
         <v>2.25</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="26">
         <v>106.06</v>
       </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26">
-        <v>0</v>
-      </c>
-      <c r="O21" s="26"/>
-      <c r="P21" s="27"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25">
+        <v>0</v>
+      </c>
+      <c r="O21" s="25"/>
+      <c r="P21" s="26"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="25">
+      <c r="A22" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="24">
         <v>3</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>133</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="31">
         <v>14</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="26">
         <v>659.94</v>
       </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26">
-        <v>0</v>
-      </c>
-      <c r="O22" s="26"/>
-      <c r="P22" s="27"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25">
+        <v>0</v>
+      </c>
+      <c r="O22" s="25"/>
+      <c r="P22" s="26"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="25">
+      <c r="A23" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="24">
         <v>3</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <v>134</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <v>1.7</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="26">
         <v>80.14</v>
       </c>
-      <c r="F23" s="32"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26">
-        <v>0</v>
-      </c>
-      <c r="O23" s="26"/>
-      <c r="P23" s="27"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25">
+        <v>0</v>
+      </c>
+      <c r="O23" s="25"/>
+      <c r="P23" s="26"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="25">
+      <c r="A24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="24">
         <v>3</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <v>135</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>1.2</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="26">
         <v>56.57</v>
       </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26">
-        <v>0</v>
-      </c>
-      <c r="O24" s="26"/>
-      <c r="P24" s="27"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25">
+        <v>0</v>
+      </c>
+      <c r="O24" s="25"/>
+      <c r="P24" s="26"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41">
+      <c r="A25" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="37">
         <f>E2+E10+E19</f>
         <v>4711.4699999999993</v>
       </c>
-      <c r="E25" s="42">
-        <f>LCMCosts!H3</f>
+      <c r="E25" s="38">
+        <f>lcmcosts_df!H3</f>
         <v>4878.569151867554</v>
       </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="42">
-        <f>LCMCosts!$H$3</f>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38">
+        <f>lcmcosts_df!$H$3</f>
         <v>4878.569151867554</v>
       </c>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="40"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="5"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="29"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2534,7 +2341,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2549,57 +2356,57 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="G1" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="H1" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="I1" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="J1" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="7">
+        <v>56</v>
+      </c>
+      <c r="C2" s="6">
         <v>12038038</v>
       </c>
       <c r="D2">
         <v>0.98</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>-0.26500000000000001</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <f t="shared" ref="G2:G32" si="0">C2*(P_^D2)*(H_^E2)</f>
         <v>97407388.003308117</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <f>G2/(P_*1000)</f>
         <v>3746.4380001272352</v>
       </c>
@@ -2612,12 +2419,12 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="7">
+        <v>57</v>
+      </c>
+      <c r="C3" s="6">
         <v>8717830</v>
       </c>
       <c r="D3">
@@ -2626,11 +2433,11 @@
       <c r="E3">
         <v>-0.12</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <f t="shared" si="0"/>
         <v>126842797.94855641</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <f t="shared" ref="H3:H7" si="1">G3/(P_*1000)</f>
         <v>4878.569151867554</v>
       </c>
@@ -2643,12 +2450,12 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="7">
+        <v>58</v>
+      </c>
+      <c r="C4" s="6">
         <v>11277566</v>
       </c>
       <c r="D4">
@@ -2657,11 +2464,11 @@
       <c r="E4">
         <v>-0.17699999999999999</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <f t="shared" si="0"/>
         <v>77872603.388702989</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <f t="shared" si="1"/>
         <v>2995.1001303347302</v>
       </c>
@@ -2674,12 +2481,12 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="7">
+        <v>59</v>
+      </c>
+      <c r="C5" s="6">
         <v>2442817</v>
       </c>
       <c r="D5">
@@ -2688,11 +2495,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <f t="shared" si="0"/>
         <v>55571276.693210892</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <f t="shared" si="1"/>
         <v>2137.3567958927265</v>
       </c>
@@ -2705,12 +2512,12 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="7">
+        <v>60</v>
+      </c>
+      <c r="C6" s="6">
         <v>3030671</v>
       </c>
       <c r="D6">
@@ -2719,11 +2526,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <f t="shared" si="0"/>
         <v>42567895.376112483</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <f t="shared" si="1"/>
         <v>1637.2267452350954</v>
       </c>
@@ -2736,12 +2543,12 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="7">
+        <v>61</v>
+      </c>
+      <c r="C7" s="6">
         <v>299461</v>
       </c>
       <c r="D7">
@@ -2750,11 +2557,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <f t="shared" si="0"/>
         <v>3481891.2409069301</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <f t="shared" si="1"/>
         <v>133.91889388103579</v>
       </c>
@@ -2767,10 +2574,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>610000</v>
@@ -2782,13 +2589,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="8">
+        <v>8</v>
+      </c>
+      <c r="G8" s="7">
         <f t="shared" si="0"/>
         <v>5967757.6557726264</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <f t="shared" ref="H8:H33" si="2">G8/(P_*1000)</f>
         <v>229.52914060663949</v>
       </c>
@@ -2801,10 +2608,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>310000</v>
@@ -2816,13 +2623,13 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="8">
+        <v>8</v>
+      </c>
+      <c r="G9" s="7">
         <f t="shared" si="0"/>
         <v>3032794.8742451053</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <f t="shared" si="2"/>
         <v>116.64595670173482</v>
       </c>
@@ -2835,10 +2642,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>210000</v>
@@ -2852,11 +2659,11 @@
       <c r="F10">
         <v>0.74</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>2054473.9470692647</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <f t="shared" si="2"/>
         <v>79.018228733433261</v>
       </c>
@@ -2869,10 +2676,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>3300000</v>
@@ -2886,11 +2693,11 @@
       <c r="F11">
         <v>0.81</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
         <v>61942674.512147166</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <f t="shared" si="2"/>
         <v>2382.4105581595063</v>
       </c>
@@ -2903,12 +2710,12 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1">
         <v>2200000</v>
       </c>
       <c r="D12">
@@ -2920,11 +2727,11 @@
       <c r="F12">
         <v>0.74</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
         <v>30800026.678421535</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <f t="shared" si="2"/>
         <v>1184.6164107085206</v>
       </c>
@@ -2937,12 +2744,12 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
         <v>1400000</v>
       </c>
       <c r="D13">
@@ -2952,13 +2759,13 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="8">
+        <v>8</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
         <v>19600016.977177341</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <f t="shared" si="2"/>
         <v>753.84680681451312</v>
       </c>
@@ -2971,12 +2778,12 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1">
         <v>310000</v>
       </c>
       <c r="D14">
@@ -2986,13 +2793,13 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="8">
+        <v>8</v>
+      </c>
+      <c r="G14" s="7">
         <f t="shared" si="0"/>
         <v>7075157.4308902901</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <f t="shared" si="2"/>
         <v>272.12143964962655</v>
       </c>
@@ -3005,12 +2812,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="2">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1">
         <v>200000</v>
       </c>
       <c r="D15">
@@ -3020,13 +2827,13 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="8">
+        <v>8</v>
+      </c>
+      <c r="G15" s="7">
         <f t="shared" si="0"/>
         <v>4564617.6973485742</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <f t="shared" si="2"/>
         <v>175.56221912879133</v>
       </c>
@@ -3039,12 +2846,12 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="2">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1">
         <v>83000</v>
       </c>
       <c r="D16">
@@ -3056,11 +2863,11 @@
       <c r="F16">
         <v>0.7</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <f t="shared" si="0"/>
         <v>1894316.3443996583</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <f t="shared" si="2"/>
         <v>72.858320938448401</v>
       </c>
@@ -3073,12 +2880,12 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="2">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1">
         <v>240000</v>
       </c>
       <c r="D17">
@@ -3088,13 +2895,13 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="8">
+        <v>8</v>
+      </c>
+      <c r="G17" s="7">
         <f t="shared" si="0"/>
         <v>5658943.9087244328</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <f t="shared" si="2"/>
         <v>217.65168879709356</v>
       </c>
@@ -3107,12 +2914,12 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="2">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1">
         <v>170000</v>
       </c>
       <c r="D18">
@@ -3122,13 +2929,13 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="8">
+        <v>8</v>
+      </c>
+      <c r="G18" s="7">
         <f t="shared" si="0"/>
         <v>4008418.60201314</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <f t="shared" si="2"/>
         <v>154.16994623127462</v>
       </c>
@@ -3141,12 +2948,12 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="2">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1">
         <v>63000</v>
       </c>
       <c r="D19">
@@ -3158,11 +2965,11 @@
       <c r="F19">
         <v>0.87</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <f t="shared" si="0"/>
         <v>1485472.7760401636</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <f t="shared" si="2"/>
         <v>57.133568309237063</v>
       </c>
@@ -3175,12 +2982,12 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="2">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
         <v>100000</v>
       </c>
       <c r="D20">
@@ -3190,13 +2997,13 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="8">
+        <v>8</v>
+      </c>
+      <c r="G20" s="7">
         <f t="shared" si="0"/>
         <v>1044193.0794695499</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <f t="shared" si="2"/>
         <v>40.16127228729038</v>
       </c>
@@ -3209,12 +3016,12 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="2">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1">
         <v>85000</v>
       </c>
       <c r="D21">
@@ -3224,13 +3031,13 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="8">
+        <v>8</v>
+      </c>
+      <c r="G21" s="7">
         <f t="shared" si="0"/>
         <v>887564.11754911754</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <f t="shared" si="2"/>
         <v>34.137081444196831</v>
       </c>
@@ -3243,12 +3050,12 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="2">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1">
         <v>63000</v>
       </c>
       <c r="D22">
@@ -3260,11 +3067,11 @@
       <c r="F22">
         <v>0.94</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <f t="shared" si="0"/>
         <v>657841.64006581646</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <f t="shared" si="2"/>
         <v>25.301601540992941</v>
       </c>
@@ -3277,12 +3084,12 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="2">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
         <v>400000</v>
       </c>
       <c r="D23">
@@ -3292,13 +3099,13 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="8">
+        <v>8</v>
+      </c>
+      <c r="G23" s="7">
         <f t="shared" si="0"/>
         <v>1677444.9034032333</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <f t="shared" si="2"/>
         <v>64.517111669355131</v>
       </c>
@@ -3311,12 +3118,12 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="2">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1">
         <v>200000</v>
       </c>
       <c r="D24">
@@ -3326,13 +3133,13 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="8">
+        <v>8</v>
+      </c>
+      <c r="G24" s="7">
         <f t="shared" si="0"/>
         <v>838722.45170161664</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <f t="shared" si="2"/>
         <v>32.258555834677566</v>
       </c>
@@ -3345,12 +3152,12 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="2">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1">
         <v>70000</v>
       </c>
       <c r="D25">
@@ -3362,11 +3169,11 @@
       <c r="F25">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="7">
         <f t="shared" si="0"/>
         <v>293552.85809556581</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="8">
         <f t="shared" si="2"/>
         <v>11.290494542137147</v>
       </c>
@@ -3379,12 +3186,12 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="2">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1">
         <v>1300000</v>
       </c>
       <c r="D26">
@@ -3396,11 +3203,11 @@
       <c r="F26">
         <v>0.99</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="7">
         <f t="shared" si="0"/>
         <v>8059877.2410171926</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="8">
         <f t="shared" si="2"/>
         <v>309.99527850066124</v>
       </c>
@@ -3413,25 +3220,25 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="5">
+        <v>31</v>
+      </c>
+      <c r="C27" s="4">
         <v>3000000</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>0.71</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>-0.42</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="7">
         <f t="shared" si="0"/>
         <v>5286360.0917839799</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="8">
         <f t="shared" si="2"/>
         <v>203.32154199169153</v>
       </c>
@@ -3444,25 +3251,25 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="5">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4">
         <v>4000000</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>0.72</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>-0.38</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="7">
         <f t="shared" si="0"/>
         <v>8599880.4054408669</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="8">
         <f t="shared" si="2"/>
         <v>330.76463097849489</v>
       </c>
@@ -3475,25 +3282,25 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="5">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4">
         <v>6000000</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>0.86</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>-0.63</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="7">
         <f t="shared" si="0"/>
         <v>7196725.6331659779</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="8">
         <f t="shared" si="2"/>
         <v>276.79713973715297</v>
       </c>
@@ -3506,25 +3313,25 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="5">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4">
         <v>3000000</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>0.65</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>-0.38</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="7">
         <f>C30*(P_^D30)*(H_^E30)</f>
         <v>5134587.2823598972</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="8">
         <f t="shared" si="2"/>
         <v>197.48412624461142</v>
       </c>
@@ -3537,28 +3344,28 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="3">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2">
         <v>24000</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>0.75</v>
       </c>
-      <c r="E31" s="4">
-        <v>0</v>
-      </c>
-      <c r="F31" s="4">
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
         <v>0.6</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="7">
         <f t="shared" si="0"/>
         <v>276338.40890394803</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="8">
         <f t="shared" si="2"/>
         <v>10.628400342459539</v>
       </c>
@@ -3571,28 +3378,28 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="3">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2">
         <v>24000</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>0.8</v>
       </c>
-      <c r="E32" s="4">
-        <v>0</v>
-      </c>
-      <c r="F32" s="4">
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
         <v>0.67</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="7">
         <f t="shared" si="0"/>
         <v>325229.49147851695</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="8">
         <f t="shared" si="2"/>
         <v>12.508826595327575</v>
       </c>
@@ -3604,36 +3411,36 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="38">
+      <c r="A33" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="34">
         <v>0.17238000000000001</v>
       </c>
-      <c r="D33" s="38">
-        <v>0</v>
-      </c>
-      <c r="E33" s="38">
-        <v>0</v>
-      </c>
-      <c r="F33" s="38">
+      <c r="D33" s="34">
+        <v>0</v>
+      </c>
+      <c r="E33" s="34">
+        <v>0</v>
+      </c>
+      <c r="F33" s="34">
         <v>1.53227</v>
       </c>
-      <c r="G33" s="39">
+      <c r="G33" s="35">
         <f>C33*AEP+F33*P_</f>
         <v>23596.600300000002</v>
       </c>
-      <c r="H33" s="39">
+      <c r="H33" s="35">
         <f t="shared" si="2"/>
         <v>0.90756155000000005</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="34">
         <v>2002</v>
       </c>
-      <c r="J33" s="38">
+      <c r="J33" s="34">
         <v>1.03</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Siteprepartion module and HydroBOSCost modeule update
</commit_message>
<xml_diff>
--- a/HydroBOSSE/project_List_30MW.xlsx
+++ b/HydroBOSSE/project_List_30MW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpoudel\PycharmProjects\hybrids_shared_infrastructure\HydroBOSSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2009A6-99B9-473E-A04E-FC2D4E064265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA586427-465F-4DFC-BAB7-3849FC05AC9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{0D60E450-1675-450E-BD0E-8D35825305C1}"/>
   </bookViews>
@@ -44,35 +44,15 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={1E9BD81B-0BB7-4D0E-ACC6-D433A2855831}</author>
-    <author>tc={9874D4CB-C558-4BFA-A3B9-8B5544961CBD}</author>
     <author>tc={BAB30A2B-D06B-49FD-84CF-D2A92E7FB953}</author>
     <author>tc={8016FF47-159C-4C80-B118-49A4482C4B40}</author>
-    <author>tc={462F28C2-F901-465B-B733-6DA7C7654688}</author>
     <author>tc={F13FCBC0-F754-4B15-80BC-397A98800CBE}</author>
     <author>tc={9CB917AC-08B2-472D-9964-408B28E59283}</author>
     <author>tc={2399C061-CD1C-4A9C-8A7D-E6560221AF84}</author>
     <author>tc={82C5412E-45A5-412F-996A-E4B1AC00862A}</author>
-    <author>tc={06A01D64-BC0C-4E6E-AC72-D7F6C669A603}</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{1E9BD81B-0BB7-4D0E-ACC6-D433A2855831}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Best guess after separating the Financial Cost; Screen shot below -original % based on multiple data source</t>
-      </text>
-    </comment>
-    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{9874D4CB-C558-4BFA-A3B9-8B5544961CBD}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Based on difference of cost between PSH (26.85%) but used 16.85 for 30 MW range</t>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="2" shapeId="0" xr:uid="{BAB30A2B-D06B-49FD-84CF-D2A92E7FB953}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{BAB30A2B-D06B-49FD-84CF-D2A92E7FB953}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -80,7 +60,7 @@
     source: B&amp;V (2012)</t>
       </text>
     </comment>
-    <comment ref="A7" authorId="3" shapeId="0" xr:uid="{8016FF47-159C-4C80-B118-49A4482C4B40}">
+    <comment ref="A7" authorId="1" shapeId="0" xr:uid="{8016FF47-159C-4C80-B118-49A4482C4B40}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -88,15 +68,7 @@
     Source: B&amp;V (2012)</t>
       </text>
     </comment>
-    <comment ref="K10" authorId="4" shapeId="0" xr:uid="{462F28C2-F901-465B-B733-6DA7C7654688}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Assigning the Level 02 sum?</t>
-      </text>
-    </comment>
-    <comment ref="A11" authorId="5" shapeId="0" xr:uid="{F13FCBC0-F754-4B15-80BC-397A98800CBE}">
+    <comment ref="A11" authorId="2" shapeId="0" xr:uid="{F13FCBC0-F754-4B15-80BC-397A98800CBE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -104,7 +76,7 @@
     IRENA(2012): The civil works for the hydropower plant construction, including any infrastructure development required to access the site and the project development costs</t>
       </text>
     </comment>
-    <comment ref="A12" authorId="6" shapeId="0" xr:uid="{9CB917AC-08B2-472D-9964-408B28E59283}">
+    <comment ref="A12" authorId="3" shapeId="0" xr:uid="{9CB917AC-08B2-472D-9964-408B28E59283}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -112,7 +84,7 @@
     EPC - includes procurement cost</t>
       </text>
     </comment>
-    <comment ref="A16" authorId="7" shapeId="0" xr:uid="{2399C061-CD1C-4A9C-8A7D-E6560221AF84}">
+    <comment ref="A16" authorId="4" shapeId="0" xr:uid="{2399C061-CD1C-4A9C-8A7D-E6560221AF84}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -120,7 +92,7 @@
     ATB20: Lesser of Annual O&amp;M = (227,000 × P^0.547) or (2.5% of CAPEX)</t>
       </text>
     </comment>
-    <comment ref="A17" authorId="8" shapeId="0" xr:uid="{82C5412E-45A5-412F-996A-E4B1AC00862A}">
+    <comment ref="A17" authorId="5" shapeId="0" xr:uid="{82C5412E-45A5-412F-996A-E4B1AC00862A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -128,20 +100,12 @@
     Edited from original - for size</t>
       </text>
     </comment>
-    <comment ref="F17" authorId="9" shapeId="0" xr:uid="{06A01D64-BC0C-4E6E-AC72-D7F6C669A603}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This cost increases with size upto 18.78% (kept 8.78) for 30 MW</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="168">
   <si>
     <t>State</t>
   </si>
@@ -602,22 +566,49 @@
     <t>Grid Connection</t>
   </si>
   <si>
-    <t>HydropBost</t>
-  </si>
-  <si>
     <t>InverterTransformer Erection</t>
   </si>
   <si>
-    <t>Management Cost</t>
-  </si>
-  <si>
     <t>Racking System Installation</t>
   </si>
   <si>
-    <t>Site Prepartion</t>
-  </si>
-  <si>
     <t>Substation Cost</t>
+  </si>
+  <si>
+    <t>Hydro Bos</t>
+  </si>
+  <si>
+    <t>Sum Row</t>
+  </si>
+  <si>
+    <t>Sum Product</t>
+  </si>
+  <si>
+    <t>Site Preparation</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Labor cost multiplier</t>
+  </si>
+  <si>
+    <t>crew_price</t>
+  </si>
+  <si>
+    <t>Hourly rate USD per hour</t>
+  </si>
+  <si>
+    <t>construction_estimator</t>
+  </si>
+  <si>
+    <t>dc_ac_ratio</t>
+  </si>
+  <si>
+    <t>switchyard_y_n</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -630,7 +621,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,6 +640,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -698,7 +696,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -792,11 +790,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -852,12 +938,20 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,20 +1272,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F1" dT="2020-07-21T22:26:12.19" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{1E9BD81B-0BB7-4D0E-ACC6-D433A2855831}">
-    <text>Best guess after separating the Financial Cost; Screen shot below -original % based on multiple data source</text>
-  </threadedComment>
-  <threadedComment ref="F4" dT="2020-07-22T22:20:57.20" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{9874D4CB-C558-4BFA-A3B9-8B5544961CBD}">
-    <text>Based on difference of cost between PSH (26.85%) but used 16.85 for 30 MW range</text>
-  </threadedComment>
   <threadedComment ref="A6" dT="2020-07-16T17:40:23.16" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{BAB30A2B-D06B-49FD-84CF-D2A92E7FB953}">
     <text>source: B&amp;V (2012)</text>
   </threadedComment>
   <threadedComment ref="A7" dT="2020-07-16T17:42:19.13" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{8016FF47-159C-4C80-B118-49A4482C4B40}">
     <text>Source: B&amp;V (2012)</text>
-  </threadedComment>
-  <threadedComment ref="K10" dT="2020-07-22T20:38:47.20" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{462F28C2-F901-465B-B733-6DA7C7654688}">
-    <text>Assigning the Level 02 sum?</text>
   </threadedComment>
   <threadedComment ref="A11" dT="2020-07-16T17:45:10.10" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{F13FCBC0-F754-4B15-80BC-397A98800CBE}">
     <text>IRENA(2012): The civil works for the hydropower plant construction, including any infrastructure development required to access the site and the project development costs</text>
@@ -1205,23 +1290,20 @@
   <threadedComment ref="A17" dT="2020-07-22T19:21:22.89" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{82C5412E-45A5-412F-996A-E4B1AC00862A}">
     <text>Edited from original - for size</text>
   </threadedComment>
-  <threadedComment ref="F17" dT="2020-07-22T22:18:53.64" personId="{EA6440DF-81DF-4078-BB3C-CA053E38A400}" id="{06A01D64-BC0C-4E6E-AC72-D7F6C669A603}">
-    <text>This cost increases with size upto 18.78% (kept 8.78) for 30 MW</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B91564F-1603-4DC5-B4A2-6AD0B294541F}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>141</v>
       </c>
@@ -1312,8 +1394,26 @@
       <c r="AD1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE1" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF1" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI1" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="AJ1" s="46" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>31</v>
       </c>
@@ -1403,6 +1503,24 @@
       </c>
       <c r="AD2">
         <v>1.03</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>100</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="46">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="46" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1412,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F00D82-0C9C-43E9-A762-C56451290467}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +1545,7 @@
     <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>122</v>
       </c>
@@ -1459,26 +1577,31 @@
         <v>152</v>
       </c>
       <c r="K1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" t="s">
         <v>153</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" t="s">
         <v>154</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P1" t="s">
         <v>155</v>
       </c>
-      <c r="N1" t="s">
-        <v>156</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>158</v>
       </c>
-      <c r="Q1" s="9"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>119</v>
       </c>
@@ -1512,9 +1635,14 @@
       <c r="M2" s="28"/>
       <c r="N2" s="28"/>
       <c r="O2" s="17"/>
-      <c r="P2" s="33"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P2" s="17"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="39">
+        <f>Q2*F2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>65</v>
       </c>
@@ -1549,9 +1677,17 @@
       <c r="O3" s="25">
         <v>1</v>
       </c>
-      <c r="P3" s="26"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P3" s="25"/>
+      <c r="Q3" s="40">
+        <f>SUM(H3:P3)</f>
+        <v>1</v>
+      </c>
+      <c r="R3" s="41">
+        <f>Q3*F3</f>
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>38</v>
       </c>
@@ -1576,7 +1712,7 @@
       </c>
       <c r="H4" s="31"/>
       <c r="I4" s="25">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -1586,9 +1722,17 @@
         <v>0</v>
       </c>
       <c r="O4" s="25"/>
-      <c r="P4" s="26"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P4" s="25"/>
+      <c r="Q4" s="40">
+        <f t="shared" ref="Q4:Q24" si="1">SUM(H4:P4)</f>
+        <v>0.05</v>
+      </c>
+      <c r="R4" s="41">
+        <f t="shared" ref="R4:R24" si="2">Q4*F4</f>
+        <v>0.84250000000000014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>66</v>
       </c>
@@ -1621,9 +1765,17 @@
         <v>0</v>
       </c>
       <c r="O5" s="25"/>
-      <c r="P5" s="26"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="25"/>
+      <c r="Q5" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>64</v>
       </c>
@@ -1656,9 +1808,17 @@
         <v>0</v>
       </c>
       <c r="O6" s="25"/>
-      <c r="P6" s="26"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="25"/>
+      <c r="Q6" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>39</v>
       </c>
@@ -1691,9 +1851,17 @@
         <v>0</v>
       </c>
       <c r="O7" s="25"/>
-      <c r="P7" s="26"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P7" s="25"/>
+      <c r="Q7" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>40</v>
       </c>
@@ -1728,9 +1896,17 @@
         <v>0</v>
       </c>
       <c r="O8" s="25"/>
-      <c r="P8" s="26"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="25"/>
+      <c r="Q8" s="40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R8" s="41">
+        <f t="shared" si="2"/>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>41</v>
       </c>
@@ -1763,9 +1939,17 @@
         <v>0</v>
       </c>
       <c r="O9" s="25"/>
-      <c r="P9" s="26"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P9" s="25"/>
+      <c r="Q9" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>120</v>
       </c>
@@ -1794,16 +1978,22 @@
       <c r="H10" s="30"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
-      <c r="K10" s="28">
-        <v>1</v>
-      </c>
+      <c r="K10" s="28"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
       <c r="O10" s="28"/>
-      <c r="P10" s="27"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P10" s="28"/>
+      <c r="Q10" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>63</v>
       </c>
@@ -1838,9 +2028,17 @@
       <c r="O11" s="25">
         <v>0.12</v>
       </c>
-      <c r="P11" s="26"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P11" s="25"/>
+      <c r="Q11" s="40">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="R11" s="41">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>42</v>
       </c>
@@ -1875,9 +2073,17 @@
         <v>0</v>
       </c>
       <c r="O12" s="25"/>
-      <c r="P12" s="26"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P12" s="25"/>
+      <c r="Q12" s="40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R12" s="41">
+        <f t="shared" si="2"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>43</v>
       </c>
@@ -1901,26 +2107,34 @@
         <v>229.29275013777504</v>
       </c>
       <c r="H13" s="31">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="25">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="K13" s="25"/>
       <c r="L13" s="25">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M13" s="25"/>
       <c r="N13" s="25">
         <v>0</v>
       </c>
       <c r="O13" s="25"/>
-      <c r="P13" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P13" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="40">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="R13" s="41">
+        <f t="shared" si="2"/>
+        <v>4.2300000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>44</v>
       </c>
@@ -1946,20 +2160,28 @@
       <c r="H14" s="31"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="M14" s="25"/>
       <c r="N14" s="25">
         <v>0</v>
       </c>
       <c r="O14" s="25"/>
-      <c r="P14" s="26"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P14" s="25"/>
+      <c r="Q14" s="40">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="R14" s="41">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>45</v>
       </c>
@@ -1994,9 +2216,17 @@
       <c r="O15" s="25">
         <v>1</v>
       </c>
-      <c r="P15" s="26"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P15" s="25"/>
+      <c r="Q15" s="40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R15" s="41">
+        <f t="shared" si="2"/>
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>46</v>
       </c>
@@ -2031,9 +2261,17 @@
         <v>0</v>
       </c>
       <c r="O16" s="25"/>
-      <c r="P16" s="26"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P16" s="25"/>
+      <c r="Q16" s="40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R16" s="41">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>47</v>
       </c>
@@ -2066,11 +2304,19 @@
         <v>0</v>
       </c>
       <c r="O17" s="25">
-        <v>1</v>
-      </c>
-      <c r="P17" s="26"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="40">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="R17" s="41">
+        <f t="shared" si="2"/>
+        <v>2.1949999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>48</v>
       </c>
@@ -2105,9 +2351,17 @@
       <c r="O18" s="25">
         <v>0.1</v>
       </c>
-      <c r="P18" s="26"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P18" s="25"/>
+      <c r="Q18" s="40">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="R18" s="41">
+        <f t="shared" si="2"/>
+        <v>5.3000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>121</v>
       </c>
@@ -2139,9 +2393,17 @@
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
       <c r="O19" s="28"/>
-      <c r="P19" s="27"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P19" s="28"/>
+      <c r="Q19" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>49</v>
       </c>
@@ -2169,9 +2431,17 @@
         <v>0</v>
       </c>
       <c r="O20" s="25"/>
-      <c r="P20" s="26"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P20" s="25"/>
+      <c r="Q20" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>50</v>
       </c>
@@ -2199,9 +2469,17 @@
         <v>0</v>
       </c>
       <c r="O21" s="25"/>
-      <c r="P21" s="26"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P21" s="25"/>
+      <c r="Q21" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>51</v>
       </c>
@@ -2229,9 +2507,17 @@
         <v>0</v>
       </c>
       <c r="O22" s="25"/>
-      <c r="P22" s="26"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P22" s="25"/>
+      <c r="Q22" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>52</v>
       </c>
@@ -2259,9 +2545,17 @@
         <v>0</v>
       </c>
       <c r="O23" s="25"/>
-      <c r="P23" s="26"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P23" s="25"/>
+      <c r="Q23" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>53</v>
       </c>
@@ -2289,44 +2583,60 @@
         <v>0</v>
       </c>
       <c r="O24" s="25"/>
-      <c r="P24" s="26"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
+      <c r="P24" s="25"/>
+      <c r="Q24" s="42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="36">
         <f>E2+E10+E19</f>
         <v>4711.4699999999993</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="37">
         <f>lcmcosts_df!H3</f>
         <v>4878.569151867554</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38">
+      <c r="F25" s="36"/>
+      <c r="G25" s="37">
         <f>lcmcosts_df!$H$3</f>
         <v>4878.569151867554</v>
       </c>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="44">
+        <f>SUM(Q2:Q24)</f>
+        <v>6.92</v>
+      </c>
+      <c r="R25" s="45">
+        <f>SUM(R2:R24)</f>
+        <v>35.230499999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
     </row>
   </sheetData>
@@ -2341,7 +2651,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,36 +3721,36 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="34">
+      <c r="C33" s="33">
         <v>0.17238000000000001</v>
       </c>
-      <c r="D33" s="34">
-        <v>0</v>
-      </c>
-      <c r="E33" s="34">
-        <v>0</v>
-      </c>
-      <c r="F33" s="34">
+      <c r="D33" s="33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="33">
         <v>1.53227</v>
       </c>
-      <c r="G33" s="35">
+      <c r="G33" s="34">
         <f>C33*AEP+F33*P_</f>
         <v>23596.600300000002</v>
       </c>
-      <c r="H33" s="35">
+      <c r="H33" s="34">
         <f t="shared" si="2"/>
         <v>0.90756155000000005</v>
       </c>
-      <c r="I33" s="34">
+      <c r="I33" s="33">
         <v>2002</v>
       </c>
-      <c r="J33" s="34">
+      <c r="J33" s="33">
         <v>1.03</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added cost modules to the HydroBOSSE
</commit_message>
<xml_diff>
--- a/HydroBOSSE/project_List_30MW.xlsx
+++ b/HydroBOSSE/project_List_30MW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpoudel\PycharmProjects\hybrids_shared_infrastructure\HydroBOSSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA586427-465F-4DFC-BAB7-3849FC05AC9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4731188-057A-4C8A-A23C-8D429B4C7434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{0D60E450-1675-450E-BD0E-8D35825305C1}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="167">
   <si>
     <t>State</t>
   </si>
@@ -476,9 +476,6 @@
     <t>1.0Initial Capital Costs (ICC)</t>
   </si>
   <si>
-    <t>2.0 Sub-Total Cost</t>
-  </si>
-  <si>
     <t>NERC Area</t>
   </si>
   <si>
@@ -572,9 +569,6 @@
     <t>Racking System Installation</t>
   </si>
   <si>
-    <t>Substation Cost</t>
-  </si>
-  <si>
     <t>Hydro Bos</t>
   </si>
   <si>
@@ -609,6 +603,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Substation</t>
   </si>
 </sst>
 </file>
@@ -652,7 +649,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -689,49 +686,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -751,43 +711,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -853,13 +776,51 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -867,12 +828,10 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -882,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -894,24 +853,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -929,29 +874,44 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1297,27 +1257,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B91564F-1603-4DC5-B4A2-6AD0B294541F}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
         <v>141</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>143</v>
-      </c>
-      <c r="D1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" t="s">
-        <v>144</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -1326,13 +1286,13 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
@@ -1341,76 +1301,76 @@
         <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
       </c>
       <c r="O1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>146</v>
+      </c>
+      <c r="R1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" t="s">
+        <v>131</v>
+      </c>
+      <c r="T1" t="s">
         <v>135</v>
       </c>
-      <c r="P1" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>147</v>
-      </c>
-      <c r="R1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S1" t="s">
-        <v>132</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
+        <v>130</v>
+      </c>
+      <c r="V1" t="s">
         <v>136</v>
       </c>
-      <c r="U1" t="s">
-        <v>131</v>
-      </c>
-      <c r="V1" t="s">
-        <v>137</v>
-      </c>
       <c r="W1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Y1" t="s">
         <v>35</v>
       </c>
       <c r="Z1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AB1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AC1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AD1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE1" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE1" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF1" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="AG1" t="s">
         <v>161</v>
       </c>
-      <c r="AF1" s="46" t="s">
+      <c r="AH1" t="s">
         <v>162</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>164</v>
-      </c>
-      <c r="AI1" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="AJ1" s="46" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
@@ -1421,7 +1381,7 @@
         <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D2">
         <v>1800</v>
@@ -1451,7 +1411,7 @@
         <v>-106.33275999999999</v>
       </c>
       <c r="M2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N2" t="s">
         <v>117</v>
@@ -1466,7 +1426,7 @@
         <v>114</v>
       </c>
       <c r="R2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S2" t="s">
         <v>118</v>
@@ -1516,11 +1476,11 @@
       <c r="AH2">
         <v>1</v>
       </c>
-      <c r="AI2" s="46">
+      <c r="AI2" s="33">
         <v>1</v>
       </c>
-      <c r="AJ2" s="46" t="s">
-        <v>167</v>
+      <c r="AJ2" s="33" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1530,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F00D82-0C9C-43E9-A762-C56451290467}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,79 +1503,80 @@
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="N1" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="R1" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="L1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" t="s">
-        <v>160</v>
-      </c>
-      <c r="N1" t="s">
-        <v>154</v>
-      </c>
-      <c r="O1" t="s">
-        <v>159</v>
-      </c>
-      <c r="P1" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="R1" t="s">
-        <v>158</v>
-      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="9">
         <v>2</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="10">
         <v>110</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="22">
         <f>SUM(D3:D9)</f>
         <v>56.999999999999993</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="19">
         <f>SUM(E3:E9)</f>
         <v>2686.87</v>
       </c>
@@ -1623,347 +1584,342 @@
         <f>SUM(F3:F9)</f>
         <v>62.79</v>
       </c>
-      <c r="G2" s="27">
-        <f t="shared" ref="G2:G18" si="0">F2*$G$25/100</f>
+      <c r="G2" s="19">
         <v>3063.2535704576371</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="39">
+      <c r="H2" s="22"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="29">
+        <f>SUM(H2:P2)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="28">
         <f>Q2*F2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="11">
         <v>3</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="12">
         <v>111</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="23">
         <v>3.27</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="18">
         <v>154.07</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="12">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G3" s="26">
-        <f>F3*$G$25/100</f>
+      <c r="G3" s="18">
         <v>224.41418098590748</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25">
-        <v>0</v>
-      </c>
-      <c r="O3" s="25">
+      <c r="H3" s="23"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17">
+        <v>0</v>
+      </c>
+      <c r="O3" s="17">
         <v>1</v>
       </c>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="40">
+      <c r="P3" s="17"/>
+      <c r="Q3" s="29">
         <f>SUM(H3:P3)</f>
         <v>1</v>
       </c>
-      <c r="R3" s="41">
+      <c r="R3" s="30">
         <f>Q3*F3</f>
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="13">
         <v>3</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="12">
         <v>112</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="23">
         <v>19.079999999999998</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="18">
         <v>899.31</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="12">
         <v>16.850000000000001</v>
       </c>
-      <c r="G4" s="26">
-        <f t="shared" si="0"/>
+      <c r="G4" s="18">
         <v>822.03890208968301</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="25">
+      <c r="H4" s="23"/>
+      <c r="I4" s="17">
         <v>0.05</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25">
-        <v>0</v>
-      </c>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="40">
-        <f t="shared" ref="Q4:Q24" si="1">SUM(H4:P4)</f>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17">
+        <v>0</v>
+      </c>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="29">
+        <f t="shared" ref="Q4:Q24" si="0">SUM(H4:P4)</f>
         <v>0.05</v>
       </c>
-      <c r="R4" s="41">
-        <f t="shared" ref="R4:R24" si="2">Q4*F4</f>
+      <c r="R4" s="30">
+        <f t="shared" ref="R4:R24" si="1">Q4*F4</f>
         <v>0.84250000000000014</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="13">
         <v>3</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="12">
         <v>113</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="23">
         <v>2.98</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="18">
         <v>140.66999999999999</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="12">
         <v>4.5199999999999996</v>
       </c>
-      <c r="G5" s="26">
-        <f t="shared" si="0"/>
+      <c r="G5" s="18">
         <v>220.51132566441342</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25">
-        <v>0</v>
-      </c>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="40">
+      <c r="H5" s="23"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17">
+        <v>0</v>
+      </c>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R5" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="13">
         <v>3</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="12">
         <v>114</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="23">
         <v>10.37</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="18">
         <v>489.01</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="12">
         <v>14.6</v>
       </c>
-      <c r="G6" s="26">
-        <f t="shared" si="0"/>
+      <c r="G6" s="18">
         <v>712.27109617266285</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25">
-        <v>0</v>
-      </c>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="40">
+      <c r="H6" s="23"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17">
+        <v>0</v>
+      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R6" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="12">
         <v>115</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="23">
         <v>11.65</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="18">
         <v>549.29999999999995</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="12">
         <v>13.4</v>
       </c>
-      <c r="G7" s="26">
-        <f t="shared" si="0"/>
+      <c r="G7" s="18">
         <v>653.72826635025228</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25">
-        <v>0</v>
-      </c>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="40">
+      <c r="H7" s="23"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17">
+        <v>0</v>
+      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R7" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="12">
         <v>116</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="23">
         <v>7.11</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="18">
         <v>334.94</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="12">
         <v>5.25</v>
       </c>
-      <c r="G8" s="26">
-        <f t="shared" si="0"/>
+      <c r="G8" s="18">
         <v>256.12488047304657</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25">
+      <c r="H8" s="23"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17">
         <v>1</v>
       </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25">
-        <v>0</v>
-      </c>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="40">
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17">
+        <v>0</v>
+      </c>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R8" s="30">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R8" s="41">
-        <f t="shared" si="2"/>
         <v>5.25</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="14">
         <v>3</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="12">
         <v>117</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="24">
         <v>2.54</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="18">
         <v>119.57</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="12">
         <v>3.57</v>
       </c>
-      <c r="G9" s="26">
-        <f t="shared" si="0"/>
+      <c r="G9" s="18">
         <v>174.16491872167168</v>
       </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25">
-        <v>0</v>
-      </c>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="40">
+      <c r="H9" s="23"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17">
+        <v>0</v>
+      </c>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R9" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="9">
         <v>2</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="10">
         <v>120</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="22">
         <f>SUM(D11:D18)</f>
         <v>20</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="19">
         <f>SUM(E11:E18)</f>
         <v>942.75999999999988</v>
       </c>
@@ -1971,673 +1927,627 @@
         <f>SUM(F11:F18)</f>
         <v>37.22</v>
       </c>
-      <c r="G10" s="27">
-        <f t="shared" si="0"/>
+      <c r="G10" s="19">
         <v>1815.8034383251036</v>
       </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="40">
+      <c r="H10" s="22"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R10" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="13">
         <v>3</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="12">
         <v>121</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="23">
         <v>2.12</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="18">
         <v>99.84</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="12">
         <v>5</v>
       </c>
-      <c r="G11" s="26">
-        <f t="shared" si="0"/>
+      <c r="G11" s="18">
         <v>243.92845759337769</v>
       </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25">
-        <v>0</v>
-      </c>
-      <c r="O11" s="25">
+      <c r="H11" s="23"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17">
+        <v>0</v>
+      </c>
+      <c r="O11" s="17">
         <v>0.12</v>
       </c>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="40">
+      <c r="P11" s="17"/>
+      <c r="Q11" s="29">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="R11" s="30">
         <f t="shared" si="1"/>
-        <v>0.12</v>
-      </c>
-      <c r="R11" s="41">
-        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="11">
         <v>3</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="12">
         <v>122</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="23">
         <v>9.85</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="18">
         <v>464.08</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="12">
         <v>13.8</v>
       </c>
-      <c r="G12" s="26">
-        <f t="shared" si="0"/>
+      <c r="G12" s="18">
         <v>673.24254295772243</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25">
+      <c r="H12" s="23"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17">
         <v>1</v>
       </c>
-      <c r="N12" s="25">
-        <v>0</v>
-      </c>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="40">
+      <c r="N12" s="17">
+        <v>0</v>
+      </c>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R12" s="30">
         <f t="shared" si="1"/>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="15">
+        <v>3</v>
+      </c>
+      <c r="C13" s="12">
+        <v>123</v>
+      </c>
+      <c r="D13" s="23">
+        <v>1.99</v>
+      </c>
+      <c r="E13" s="18">
+        <v>93.85</v>
+      </c>
+      <c r="F13" s="12">
+        <v>4.7</v>
+      </c>
+      <c r="G13" s="18">
+        <v>229.29275013777504</v>
+      </c>
+      <c r="H13" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17">
+        <v>0</v>
+      </c>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="29">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="R13" s="30">
+        <f t="shared" si="1"/>
+        <v>4.2300000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="12">
+        <v>124</v>
+      </c>
+      <c r="D14" s="23">
+        <v>0.64</v>
+      </c>
+      <c r="E14" s="18">
+        <v>29.93</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="18">
+        <v>73.178537278013309</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17">
+        <v>0</v>
+      </c>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="29">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="R14" s="30">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="13">
+        <v>3</v>
+      </c>
+      <c r="C15" s="12">
+        <v>125</v>
+      </c>
+      <c r="D15" s="23">
+        <v>1.02</v>
+      </c>
+      <c r="E15" s="18">
+        <v>48.13</v>
+      </c>
+      <c r="F15" s="12">
+        <v>2.41</v>
+      </c>
+      <c r="G15" s="18">
+        <v>117.57351656000806</v>
+      </c>
+      <c r="H15" s="23"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17">
+        <v>0</v>
+      </c>
+      <c r="O15" s="17">
         <v>1</v>
       </c>
-      <c r="R12" s="41">
-        <f t="shared" si="2"/>
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="23">
+      <c r="P15" s="17"/>
+      <c r="Q15" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R15" s="30">
+        <f t="shared" si="1"/>
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="16">
         <v>3</v>
       </c>
-      <c r="C13" s="20">
-        <v>123</v>
-      </c>
-      <c r="D13" s="31">
-        <v>1.99</v>
-      </c>
-      <c r="E13" s="26">
-        <v>93.85</v>
-      </c>
-      <c r="F13">
-        <v>4.7</v>
-      </c>
-      <c r="G13" s="26">
-        <f t="shared" si="0"/>
-        <v>229.29275013777504</v>
-      </c>
-      <c r="H13" s="31">
-        <v>0.1</v>
-      </c>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25">
-        <v>0</v>
-      </c>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25">
+      <c r="C16" s="12">
+        <v>126</v>
+      </c>
+      <c r="D16" s="23">
+        <v>0.21</v>
+      </c>
+      <c r="E16" s="18">
+        <v>9.99</v>
+      </c>
+      <c r="F16" s="12">
         <v>0.5</v>
       </c>
-      <c r="Q13" s="40">
-        <f t="shared" si="1"/>
-        <v>0.9</v>
-      </c>
-      <c r="R13" s="41">
-        <f t="shared" si="2"/>
-        <v>4.2300000000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="22">
-        <v>3</v>
-      </c>
-      <c r="C14" s="20">
-        <v>124</v>
-      </c>
-      <c r="D14" s="31">
-        <v>0.64</v>
-      </c>
-      <c r="E14" s="26">
-        <v>29.93</v>
-      </c>
-      <c r="F14">
-        <v>1.5</v>
-      </c>
-      <c r="G14" s="26">
-        <f t="shared" si="0"/>
-        <v>73.178537278013309</v>
-      </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25">
-        <v>0</v>
-      </c>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="40">
+      <c r="G16" s="18">
+        <v>24.392845759337771</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17">
+        <v>1</v>
+      </c>
+      <c r="N16" s="17">
+        <v>0</v>
+      </c>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R16" s="30">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="R14" s="41">
-        <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="21">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="13">
         <v>3</v>
       </c>
-      <c r="C15" s="20">
-        <v>125</v>
-      </c>
-      <c r="D15" s="31">
-        <v>1.02</v>
-      </c>
-      <c r="E15" s="26">
-        <v>48.13</v>
-      </c>
-      <c r="F15">
-        <v>2.41</v>
-      </c>
-      <c r="G15" s="26">
-        <f t="shared" si="0"/>
-        <v>117.57351656000806</v>
-      </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25">
-        <v>0</v>
-      </c>
-      <c r="O15" s="25">
-        <v>1</v>
-      </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="40">
+      <c r="C17" s="12">
+        <v>127</v>
+      </c>
+      <c r="D17" s="23">
+        <v>3.95</v>
+      </c>
+      <c r="E17" s="18">
+        <v>186.38</v>
+      </c>
+      <c r="F17" s="12">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="G17" s="18">
+        <v>428.33837153397121</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17">
+        <v>0</v>
+      </c>
+      <c r="O17" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="29">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="R17" s="30">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R15" s="41">
-        <f t="shared" si="2"/>
-        <v>2.41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="24">
+        <v>2.1949999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="13">
         <v>3</v>
       </c>
-      <c r="C16" s="20">
-        <v>126</v>
-      </c>
-      <c r="D16" s="31">
-        <v>0.21</v>
-      </c>
-      <c r="E16" s="26">
-        <v>9.99</v>
-      </c>
-      <c r="F16">
-        <v>0.5</v>
-      </c>
-      <c r="G16" s="26">
-        <f t="shared" si="0"/>
-        <v>24.392845759337771</v>
-      </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25">
-        <v>1</v>
-      </c>
-      <c r="N16" s="25">
-        <v>0</v>
-      </c>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="40">
+      <c r="C18" s="12">
+        <v>128</v>
+      </c>
+      <c r="D18" s="23">
+        <v>0.22</v>
+      </c>
+      <c r="E18" s="18">
+        <v>10.56</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0.53</v>
+      </c>
+      <c r="G18" s="18">
+        <v>25.856416504898039</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17">
+        <v>0</v>
+      </c>
+      <c r="O18" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="29">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="R18" s="30">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R16" s="41">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="21">
-        <v>3</v>
-      </c>
-      <c r="C17" s="20">
-        <v>127</v>
-      </c>
-      <c r="D17" s="31">
-        <v>3.95</v>
-      </c>
-      <c r="E17" s="26">
-        <v>186.38</v>
-      </c>
-      <c r="F17">
-        <v>8.7799999999999994</v>
-      </c>
-      <c r="G17" s="26">
-        <f t="shared" si="0"/>
-        <v>428.33837153397121</v>
-      </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25">
-        <v>0</v>
-      </c>
-      <c r="O17" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="40">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="R17" s="41">
-        <f t="shared" si="2"/>
-        <v>2.1949999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="21">
-        <v>3</v>
-      </c>
-      <c r="C18" s="20">
-        <v>128</v>
-      </c>
-      <c r="D18" s="31">
-        <v>0.22</v>
-      </c>
-      <c r="E18" s="26">
-        <v>10.56</v>
-      </c>
-      <c r="F18">
-        <v>0.53</v>
-      </c>
-      <c r="G18" s="26">
-        <f t="shared" si="0"/>
-        <v>25.856416504898039</v>
-      </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25">
-        <v>0</v>
-      </c>
-      <c r="O18" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="40">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="R18" s="41">
-        <f t="shared" si="2"/>
         <v>5.3000000000000005E-2</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="9">
         <v>2</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="10">
         <v>130</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="22">
         <f>SUM(D20:D24)</f>
         <v>22.95</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="19">
         <f>SUM(E20:E24)</f>
         <v>1081.8400000000001</v>
       </c>
-      <c r="F19" s="30">
-        <v>0</v>
-      </c>
-      <c r="G19" s="27">
-        <v>0</v>
-      </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="40">
+      <c r="F19" s="22">
+        <v>0</v>
+      </c>
+      <c r="G19" s="19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R19" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="16">
         <v>3</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="12">
         <v>131</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="23">
         <v>3.8</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="18">
         <v>179.13</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25">
-        <v>0</v>
-      </c>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="40">
+      <c r="F20" s="23"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17">
+        <v>0</v>
+      </c>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R20" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="16">
         <v>3</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="12">
         <v>132</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="23">
         <v>2.25</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="18">
         <v>106.06</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25">
-        <v>0</v>
-      </c>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="40">
+      <c r="F21" s="23"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17">
+        <v>0</v>
+      </c>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R21" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="24">
+      <c r="B22" s="16">
         <v>3</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="12">
         <v>133</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="23">
         <v>14</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="18">
         <v>659.94</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25">
-        <v>0</v>
-      </c>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="40">
+      <c r="F22" s="23"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17">
+        <v>0</v>
+      </c>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R22" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="16">
         <v>3</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="12">
         <v>134</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="23">
         <v>1.7</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="18">
         <v>80.14</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25">
-        <v>0</v>
-      </c>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="40">
+      <c r="F23" s="23"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17">
+        <v>0</v>
+      </c>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R23" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="41">
         <v>3</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="42">
         <v>135</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="43">
         <v>1.2</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="44">
         <v>56.57</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25">
-        <v>0</v>
-      </c>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="42">
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45">
+        <v>0</v>
+      </c>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R24" s="43">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="36">
-        <f>E2+E10+E19</f>
-        <v>4711.4699999999993</v>
-      </c>
-      <c r="E25" s="37">
-        <f>lcmcosts_df!H3</f>
-        <v>4878.569151867554</v>
-      </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="37">
-        <f>lcmcosts_df!$H$3</f>
-        <v>4878.569151867554</v>
-      </c>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="44">
-        <f>SUM(Q2:Q24)</f>
-        <v>6.92</v>
-      </c>
-      <c r="R25" s="45">
-        <f>SUM(R2:R24)</f>
-        <v>35.230499999999999</v>
-      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="A26" s="21"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="A27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3721,36 +3631,36 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="33">
+      <c r="C33" s="25">
         <v>0.17238000000000001</v>
       </c>
-      <c r="D33" s="33">
-        <v>0</v>
-      </c>
-      <c r="E33" s="33">
-        <v>0</v>
-      </c>
-      <c r="F33" s="33">
+      <c r="D33" s="25">
+        <v>0</v>
+      </c>
+      <c r="E33" s="25">
+        <v>0</v>
+      </c>
+      <c r="F33" s="25">
         <v>1.53227</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="26">
         <f>C33*AEP+F33*P_</f>
         <v>23596.600300000002</v>
       </c>
-      <c r="H33" s="34">
+      <c r="H33" s="26">
         <f t="shared" si="2"/>
         <v>0.90756155000000005</v>
       </c>
-      <c r="I33" s="33">
+      <c r="I33" s="25">
         <v>2002</v>
       </c>
-      <c r="J33" s="33">
+      <c r="J33" s="25">
         <v>1.03</v>
       </c>
     </row>

</xml_diff>